<commit_message>
benchmark product list update
</commit_message>
<xml_diff>
--- a/benchmark/Mobile_manipulator_product_list.xlsx
+++ b/benchmark/Mobile_manipulator_product_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nswve\OneDrive\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nswve\Dropbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17685"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="HARDWARE" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Product list</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,26 +42,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Motor(ARM)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Motor(BASE)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MCU</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Audio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB Hub</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Depth Cam</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -98,23 +82,211 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Accelerometer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slamtex RPLidar A1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intel NUC-8 I5-8259U/RAM:16GB/SSD:500GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D435 with IMU (D435i)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pan range of motion : 346 deg
+Tilt range of motion : 115 deg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motor(WRIST-PCBA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motor(BASE-PCBA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motor(HEAD-PCBA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Motor(SHOULDER-PCBA)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamixel XL430 x 2
+Arm Controller : Atmel SAMD21G18 x 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arm Controller : Atmel SAMD21G18 x 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 inch diameter, urethane rubber shore 60A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diameter 50mm</t>
+  </si>
+  <si>
+    <t>Ethernet Port</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connected to computer NIC</t>
+  </si>
+  <si>
+    <t>USB HUB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>light on when its on</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery charger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rated for upplied 12V/7A charger</t>
+  </si>
+  <si>
+    <t>HDMI Port</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connected to computer HDMI</t>
+  </si>
+  <si>
+    <t>Wheel Stepper Controller : Atmel SAMD21G18 x 3
+Lift Stepper Controller : Atmel SAMD21G18 x 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timing belt for lift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gripper</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamixel XL430 x 2
+Arm Controller : Atmel SAMD21G18 x 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamixel XL430 x 2</t>
+  </si>
+  <si>
     <t>Charger</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Motor(CAM)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mircophone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Accelerometer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>timing belt</t>
+    <t>6 Port USB Hub - USB 3.0 , powered 5V/3A
+4 Port USB-3 Hub for Atmel Controller  x 3
+7 Port USB-3 Hub for User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nvidia Jetson NX(석훈)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dynamixel XL430 x 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Base Motor(인휠 드라이버)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenCR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sharp GP2Y0A51SK0F, Analog, range 2-15 cm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMG Button/ On off Button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batter 선정할 때 고민해야 함/메인 분배기 선정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호연이/현준이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스텝 모터/타이밍 밸트/효재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효재</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9DOF FXOS8700 + FXAS21002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>링크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slamtex RPLidar A2-A3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 : https://www.devicemart.co.kr/goods/view?no=12498793#goods_file
+3D 모델 : https://www.slamtec.com/en/Support#rplidar-a2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 : http://vctec.co.kr/product/9dof-imu%EC%84%BC%EC%84%9C-fxos8700-fxas21002-adafruit-precision-nxp-9-dof-breakout-bo/11435/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intel D455</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D 모델 : https://dev.intelrealsense.com/docs/cad-files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D 모델 : https://github.com/ROBOTIS-GIT/OpenCR-Hardware</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 DOF ADXL343</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매 : https://www.icbanq.com/P007406244
+3D 모델 : https://grabcad.com/library/adxl345-digital-accelerometer-adafuit-breakout-board-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판매 : https://www.robotis.com/shop/item.php?it_id=902-0135-000
+3D 모델 : https://emanual.robotis.com/docs/kr/dxl/x/xl430-w250/#%EB%8F%84%EB%A9%B4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -122,7 +294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +339,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -185,12 +373,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -203,12 +394,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,17 +714,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="20.625" customWidth="1"/>
+    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="2" max="2" width="42.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="122.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -509,7 +738,9 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -529,111 +760,271 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="C2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:18" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="33" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="17.25" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D3:D5"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" display="http://vctec.co.kr/product/9dof-imu%EC%84%BC%EC%84%9C-fxos8700-fxas21002-adafruit-precision-nxp-9-dof-breakout-bo/11435/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>